<commit_message>
flattening with explicit id and name
</commit_message>
<xml_diff>
--- a/examples/flat_annotation.xlsx
+++ b/examples/flat_annotation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>display_id</t>
   </si>
@@ -27,24 +27,9 @@
     <t>description</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
-    <t>slr0612</t>
-  </si>
-  <si>
-    <t>slr0613</t>
-  </si>
-  <si>
-    <t>sll0558</t>
-  </si>
-  <si>
-    <t>{key}_codA_flat</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -54,10 +39,16 @@
     <t>assembled on 2021-06-10</t>
   </si>
   <si>
-    <t>"flattened version" of the design suitable for visualization and genbank export</t>
-  </si>
-  <si>
-    <t>{key}-codA</t>
+    <t>cs0002_slr0612</t>
+  </si>
+  <si>
+    <t>cs0003_slr0613</t>
+  </si>
+  <si>
+    <t>cs0004_sll0558</t>
+  </si>
+  <si>
+    <t>"flattened version" of the design {key} suitable for visualization and genbank export</t>
   </si>
 </sst>
 </file>
@@ -375,80 +366,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE(A2,"_flat")</f>
+        <v>cs0002_slr0612_flat</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B4" si="0">CONCATENATE(A3,"_flat")</f>
+        <v>cs0003_slr0613_flat</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>cs0004_sll0558_flat</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>